<commit_message>
commonName: A1#111DHARMAHEALTHCAREXX subject_application_id: HNRIS subject_application_vendor: DHARMA subject_application_version: 0.1
Corretto il file checklist come richiesto
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DHARMAHEALTHCAREXX/DHARMA/HNRIS/0.1/accreditamento-checklist.xlsx
+++ b/GATEWAY/A1#111DHARMAHEALTHCAREXX/DHARMA/HNRIS/0.1/accreditamento-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raffa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF4C288-5665-4C62-8A38-579DC0B4CBE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9404841-870C-4FEE-B579-5579E735213A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="196">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2890,7 +2890,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3625,7 +3625,9 @@
       <c r="P17" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="Q17" s="29"/>
+      <c r="Q17" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="R17" s="29" t="s">
         <v>83</v>
       </c>
@@ -10741,27 +10743,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -11019,32 +11000,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11061,4 +11038,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ricaricati file di test
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DHARMAHEALTHCAREXX/DHARMA/HNRIS/0.1/accreditamento-checklist.xlsx
+++ b/GATEWAY/A1#111DHARMAHEALTHCAREXX/DHARMA/HNRIS/0.1/accreditamento-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raffa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2246205A-FAFC-469B-A877-5319A5CB46A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0E6934-5E8C-4D9A-9B07-EDD21A638021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -825,13 +825,13 @@
     <t>Errore di sintassi: ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{\"urn:hl7-org:v3\":languageCode}'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected.</t>
   </si>
   <si>
-    <t>2025-06-19T14:26:40Z</t>
-  </si>
-  <si>
-    <t>633c87ae7985a0fd71cf297bc1c50fda</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.37165d2e4c0a943485b755b229ae923c77d4dcaf62c02274c6cdb64b359900cf.1a23547554^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-25T08:49:57Z</t>
+  </si>
+  <si>
+    <t>96b420b065a7f1c01874ea35eed49580</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.72421086d62e3cc2bf95c2fbf883e816587b312510c4839aad1d815dbe90e1a0.92b140d03e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2898,7 +2898,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4218,7 +4218,7 @@
         <v>105</v>
       </c>
       <c r="F30" s="33">
-        <v>45827</v>
+        <v>45833</v>
       </c>
       <c r="G30" s="33" t="s">
         <v>193</v>
@@ -10751,6 +10751,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
@@ -10760,15 +10769,6 @@
     <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11030,6 +11030,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -11042,14 +11050,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Nuovo invio files Test checklist e data.json
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DHARMAHEALTHCAREXX/DHARMA/HNRIS/0.1/accreditamento-checklist.xlsx
+++ b/GATEWAY/A1#111DHARMAHEALTHCAREXX/DHARMA/HNRIS/0.1/accreditamento-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raffa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0E6934-5E8C-4D9A-9B07-EDD21A638021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EE2F8E-6BD8-493A-8F9D-5FD859F3E1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -825,13 +825,13 @@
     <t>Errore di sintassi: ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{\"urn:hl7-org:v3\":languageCode}'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected.</t>
   </si>
   <si>
-    <t>2025-06-25T08:49:57Z</t>
-  </si>
-  <si>
-    <t>96b420b065a7f1c01874ea35eed49580</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.72421086d62e3cc2bf95c2fbf883e816587b312510c4839aad1d815dbe90e1a0.92b140d03e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.ea5fc7867f7a91b95c9cc4cc874fda845bc8fdc4304ef808a8593dee89bfa584.1c35c60ee8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e97bc80087521153f347dc7ca39932ff</t>
+  </si>
+  <si>
+    <t>2025-06-29T21:26:19Z</t>
   </si>
 </sst>
 </file>
@@ -4218,16 +4218,16 @@
         <v>105</v>
       </c>
       <c r="F30" s="33">
-        <v>45833</v>
+        <v>45837</v>
       </c>
       <c r="G30" s="33" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H30" s="33" t="s">
         <v>194</v>
       </c>
       <c r="I30" s="37" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J30" s="29" t="s">
         <v>51</v>
@@ -8479,8 +8479,8 @@
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -10751,27 +10751,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -11029,10 +11008,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11055,20 +11066,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>